<commit_message>
Adding sch related words graphs and results
</commit_message>
<xml_diff>
--- a/resultsDump/featureTTestResults.xlsx
+++ b/resultsDump/featureTTestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>rhyme</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>yngve</t>
+  </si>
+  <si>
+    <t>schcount</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,109 +943,144 @@
         <v>0.2437</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.8983000000000003E-7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>5.3E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1.5543999999999999E-4</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>6.016E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
         <v>1.8434E-5</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
         <v>1.4721E-5</v>
       </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0.37890000000000001</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>0.83650000000000002</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>0.28120000000000001</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>0.52210000000000001</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
         <v>5.5309999999999995E-4</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>0.81259999999999999</v>
       </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>2.52E-2</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>0.87490000000000001</v>
       </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
-      <c r="K15">
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>0.61329999999999996</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
         <v>0.27860000000000001</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>0.38929999999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding some results pics
</commit_message>
<xml_diff>
--- a/resultsDump/featureTTestResults.xlsx
+++ b/resultsDump/featureTTestResults.xlsx
@@ -149,10 +149,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -461,7 +462,7 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,6 +978,18 @@
       <c r="K13" s="1">
         <v>6.016E-5</v>
       </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1.0011E-4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>3.5000000000000001E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Add neologism results and graphs
</commit_message>
<xml_diff>
--- a/resultsDump/featureTTestResults.xlsx
+++ b/resultsDump/featureTTestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>rhyme</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>cpidr</t>
+  </si>
+  <si>
+    <t>neologism</t>
   </si>
 </sst>
 </file>
@@ -464,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +997,17 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>

</xml_diff>